<commit_message>
updates to bsdf model and rules
</commit_message>
<xml_diff>
--- a/seeddata-bsdf/99-exceldmd/Authorization Model.xlsx
+++ b/seeddata-bsdf/99-exceldmd/Authorization Model.xlsx
@@ -50,8 +50,8 @@
   </definedNames>
   <calcPr calcId="145621" iterateDelta="1E-4" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Gupta, Kunal - Personal View" guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" tabRatio="500" activeSheetId="4"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" mergeInterval="0" personalView="1" windowWidth="1472" windowHeight="548" tabRatio="500" activeSheetId="4"/>
-    <customWorkbookView name="Gupta, Kunal - Personal View" guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" tabRatio="500" activeSheetId="4"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="115">
   <si>
     <t>ACTION</t>
   </si>
@@ -997,17 +997,7 @@
     <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1439,12 +1429,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1545,12 +1535,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}">
+      <selection activeCell="B34" sqref="B34"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}">
       <selection activeCell="A5" sqref="A5"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}">
-      <selection activeCell="B34" sqref="B34"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -1696,11 +1686,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -1837,14 +1827,14 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="150">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="150">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="150">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -1856,11 +1846,11 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2386,37 +2376,11 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="H20" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="I20" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="J20" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="K20" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L20" s="23" t="s">
-        <v>89</v>
-      </c>
-    </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B322" sqref="B322"/>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1" topLeftCell="E1">
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
       <colBreaks count="1" manualBreakCount="1">
         <brk id="2" max="1048575" man="1"/>
       </colBreaks>
@@ -2424,9 +2388,9 @@
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A1:AE347"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1" topLeftCell="E1">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B322" sqref="B322"/>
       <colBreaks count="1" manualBreakCount="1">
         <brk id="2" max="1048575" man="1"/>
       </colBreaks>
@@ -2842,7 +2806,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G21">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2901,12 +2865,12 @@
     <sortCondition ref="B2"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3004,12 +2968,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3020,65 +2984,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003CF273DB610BE64D8338C714685CCF46" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2352d1590348b4df6d1de565ccbd102a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fff5a07-2326-481b-a4e9-87ff7a79f8dd" xmlns:ns3="2e2046eb-f52d-433a-aad8-97c651e3992c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5c0a0cba47b5c64de8255dd546e4ec9" ns2:_="" ns3:_="">
     <xsd:import namespace="0fff5a07-2326-481b-a4e9-87ff7a79f8dd"/>
@@ -3256,7 +3161,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_dlc_DocId xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">Z7QZ4QWJDNQ7-73874190-24</_dlc_DocId>
@@ -3268,23 +3173,66 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{544FA98A-5D89-41A3-B3E3-9D6D7A4BCA0D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A58437D0-211E-4689-9BB7-1D7150BF8997}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CAC4C16-FDF5-437E-A8C4-D650CA39502E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3303,7 +3251,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E9ADEF4-6C25-4BA4-9EDB-E28F722B8411}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3311,4 +3259,20 @@
     <ds:schemaRef ds:uri="0fff5a07-2326-481b-a4e9-87ff7a79f8dd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{544FA98A-5D89-41A3-B3E3-9D6D7A4BCA0D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A58437D0-211E-4689-9BB7-1D7150BF8997}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>